<commit_message>
💫 Capitalizar nombres de puntos para extraerlos desde acá
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos CEPER puntos primera capa.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos CEPER puntos primera capa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/la_guzman_uniandes_edu_co/Documents/Corredor Verde 7/Diseminación de resultados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\dev\enflujo\070-cra7\aplicaciones\procesador\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{800EF7C4-7BB8-4701-A446-C41B5CF030C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554BCC63-21A0-434B-A04F-D1359FE7B71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39285" yWindow="420" windowWidth="35385" windowHeight="15705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,124 +86,16 @@
     <t xml:space="preserve">Plaza Bolivar </t>
   </si>
   <si>
-    <t>avenida jiménez</t>
-  </si>
-  <si>
     <t xml:space="preserve">Calle 19 </t>
   </si>
   <si>
     <t xml:space="preserve">Calle 26 </t>
   </si>
   <si>
-    <t>calle 32</t>
-  </si>
-  <si>
-    <t>calle 37</t>
-  </si>
-  <si>
     <t>Diagonal 40A</t>
   </si>
   <si>
     <t xml:space="preserve">Calle 45 </t>
-  </si>
-  <si>
-    <t>calle 53</t>
-  </si>
-  <si>
-    <t>calle 56</t>
-  </si>
-  <si>
-    <t>calle 60</t>
-  </si>
-  <si>
-    <t>calle 67</t>
-  </si>
-  <si>
-    <t>calle 70</t>
-  </si>
-  <si>
-    <t>calle 72</t>
-  </si>
-  <si>
-    <t>calle 74</t>
-  </si>
-  <si>
-    <t>calle 76</t>
-  </si>
-  <si>
-    <t>calle 84</t>
-  </si>
-  <si>
-    <t>calle 85</t>
-  </si>
-  <si>
-    <t>calle 92</t>
-  </si>
-  <si>
-    <t>calle 94</t>
-  </si>
-  <si>
-    <t>calle 100</t>
-  </si>
-  <si>
-    <t>calle 106</t>
-  </si>
-  <si>
-    <t>calle 116</t>
-  </si>
-  <si>
-    <t>calle 127</t>
-  </si>
-  <si>
-    <t>calle 134</t>
-  </si>
-  <si>
-    <t>calle 140</t>
-  </si>
-  <si>
-    <t>calle 147</t>
-  </si>
-  <si>
-    <t>calle 151</t>
-  </si>
-  <si>
-    <t>calle 153</t>
-  </si>
-  <si>
-    <t>calle 160</t>
-  </si>
-  <si>
-    <t>calle 164</t>
-  </si>
-  <si>
-    <t>calle 165</t>
-  </si>
-  <si>
-    <t>calle 170</t>
-  </si>
-  <si>
-    <t>calle 175</t>
-  </si>
-  <si>
-    <t>calle 180</t>
-  </si>
-  <si>
-    <t>calle 183</t>
-  </si>
-  <si>
-    <t>calle 189</t>
-  </si>
-  <si>
-    <t>calle 192</t>
-  </si>
-  <si>
-    <t>calle 193</t>
-  </si>
-  <si>
-    <t>calle 200</t>
-  </si>
-  <si>
-    <t>calle 220</t>
   </si>
   <si>
     <t xml:space="preserve">Datos </t>
@@ -3751,13 +3643,121 @@
   </si>
   <si>
     <t>7#187: "Estos largos tiempos de espera en un trancón ocasionan mucha fatiga, mucho cansancio, mucho estrés, perdida de tiempo, afectan notoriamente la calidad de vida de las personas porque si uno va sentado llega tieso a donde va a llegar, con dolor de espalda, de cuello, de piernas. Si va de pie pues la espera es eterna y el dolor de piernas es enorme. Adicional, no tiene uno tiempo de pensar en cultura, recreación, vida familiar, ni en descanso, ni en estudiar, tiempo de calidad. Se le va la mitad de tiempo del día en traslados. "</t>
+  </si>
+  <si>
+    <t>Avenida Jiménez</t>
+  </si>
+  <si>
+    <t>Calle 32</t>
+  </si>
+  <si>
+    <t>Calle 37</t>
+  </si>
+  <si>
+    <t>Calle 53</t>
+  </si>
+  <si>
+    <t>Calle 56</t>
+  </si>
+  <si>
+    <t>Calle 60</t>
+  </si>
+  <si>
+    <t>Calle 67</t>
+  </si>
+  <si>
+    <t>Calle 70</t>
+  </si>
+  <si>
+    <t>Calle 72</t>
+  </si>
+  <si>
+    <t>Calle 74</t>
+  </si>
+  <si>
+    <t>Calle 76</t>
+  </si>
+  <si>
+    <t>Calle 84</t>
+  </si>
+  <si>
+    <t>Calle 85</t>
+  </si>
+  <si>
+    <t>Calle 92</t>
+  </si>
+  <si>
+    <t>Calle 94</t>
+  </si>
+  <si>
+    <t>Calle 100</t>
+  </si>
+  <si>
+    <t>Calle 106</t>
+  </si>
+  <si>
+    <t>Calle 116</t>
+  </si>
+  <si>
+    <t>Calle 127</t>
+  </si>
+  <si>
+    <t>Calle 134</t>
+  </si>
+  <si>
+    <t>Calle 140</t>
+  </si>
+  <si>
+    <t>Calle 147</t>
+  </si>
+  <si>
+    <t>Calle 151</t>
+  </si>
+  <si>
+    <t>Calle 153</t>
+  </si>
+  <si>
+    <t>Calle 160</t>
+  </si>
+  <si>
+    <t>Calle 164</t>
+  </si>
+  <si>
+    <t>Calle 165</t>
+  </si>
+  <si>
+    <t>Calle 170</t>
+  </si>
+  <si>
+    <t>Calle 175</t>
+  </si>
+  <si>
+    <t>Calle 180</t>
+  </si>
+  <si>
+    <t>Calle 183</t>
+  </si>
+  <si>
+    <t>Calle 189</t>
+  </si>
+  <si>
+    <t>Calle 192</t>
+  </si>
+  <si>
+    <t>Calle 193</t>
+  </si>
+  <si>
+    <t>Calle 200</t>
+  </si>
+  <si>
+    <t>Calle 220</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3987,9 +3987,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3999,9 +4002,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4238,13 +4238,13 @@
   <dimension ref="A1:AV25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AA6" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AB9" sqref="AB9:AJ9"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="AO3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="AU5" sqref="AU5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="3" width="18.42578125" style="6" customWidth="1"/>
@@ -4254,7 +4254,7 @@
     <col min="7" max="47" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="12.75">
+    <row r="1" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4266,27 +4266,27 @@
       <c r="G1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="29"/>
       <c r="O1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="33"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="29"/>
       <c r="AA1" s="25" t="s">
         <v>3</v>
       </c>
@@ -4312,7 +4312,7 @@
       <c r="AU1" s="24"/>
       <c r="AV1" s="1"/>
     </row>
-    <row r="2" spans="1:48" ht="26.25" customHeight="1">
+    <row r="2" spans="1:48" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -4333,423 +4333,423 @@
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>17</v>
+        <v>195</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>18</v>
+        <v>196</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>19</v>
+        <v>197</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>20</v>
+        <v>198</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>22</v>
+        <v>200</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>23</v>
+        <v>201</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>24</v>
+        <v>202</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>25</v>
+        <v>203</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>26</v>
+        <v>204</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>27</v>
+        <v>205</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>28</v>
+        <v>206</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>29</v>
+        <v>207</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>30</v>
+        <v>208</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>31</v>
+        <v>209</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>32</v>
+        <v>210</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>33</v>
+        <v>211</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>34</v>
+        <v>212</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>35</v>
+        <v>213</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>36</v>
+        <v>214</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>37</v>
+        <v>215</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>38</v>
+        <v>216</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>39</v>
+        <v>217</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>40</v>
+        <v>218</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>41</v>
+        <v>219</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>42</v>
+        <v>220</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>43</v>
+        <v>221</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>44</v>
+        <v>222</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>45</v>
+        <v>223</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>46</v>
+        <v>224</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>47</v>
+        <v>225</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>48</v>
+        <v>226</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>49</v>
+        <v>227</v>
       </c>
       <c r="AV2" s="1"/>
     </row>
-    <row r="3" spans="1:48" ht="24">
-      <c r="A3" s="28" t="s">
-        <v>50</v>
+    <row r="3" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="6" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="U3" s="21" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="V3" s="21" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="W3" s="21" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="X3" s="21" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="Z3" s="21" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="AA3" s="21" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AB3" s="21" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AC3" s="21" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AD3" s="21" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="AE3" s="21" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="AF3" s="21" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="AG3" s="21" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="AH3" s="21" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AI3" s="21" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="AJ3" s="21" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="AK3" s="21" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="AL3" s="21" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="AM3" s="21" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="AN3" s="21" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="AO3" s="21" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="AP3" s="21" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="AQ3" s="21" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="AR3" s="21" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="AS3" s="21" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="AT3" s="21" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="AU3" s="21" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:48" ht="24">
-      <c r="A4" s="34"/>
+    <row r="4" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="31"/>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="6" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="Y4" s="21" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="Z4" s="21" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="AA4" s="21" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AB4" s="21" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="AC4" s="21" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="AD4" s="21" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="AE4" s="21" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="AF4" s="21" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="AG4" s="21" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="AH4" s="21" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="AI4" s="21" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="AJ4" s="21" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="AK4" s="21" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="AL4" s="21" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="AM4" s="21" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="AN4" s="21" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="AO4" s="21" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="AP4" s="21" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="AQ4" s="21" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="AR4" s="21" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="AS4" s="21" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="AT4" s="21" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="AU4" s="21" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:48" s="13" customFormat="1" ht="72">
-      <c r="A5" s="34"/>
+    <row r="5" spans="1:48" s="13" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="31"/>
       <c r="B5" s="12" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4757,16 +4757,16 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="P5" s="12"/>
       <c r="Q5" s="12" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
@@ -4775,13 +4775,13 @@
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
       <c r="AA5" s="12"/>
       <c r="AB5" s="12" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="AC5" s="12"/>
       <c r="AD5" s="12"/>
@@ -4803,245 +4803,245 @@
       <c r="AT5" s="12"/>
       <c r="AU5" s="12"/>
     </row>
-    <row r="6" spans="1:48" s="13" customFormat="1" ht="177">
-      <c r="A6" s="34"/>
+    <row r="6" spans="1:48" s="13" customFormat="1" ht="204" x14ac:dyDescent="0.2">
+      <c r="A6" s="31"/>
       <c r="B6" s="14" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="F6" s="15"/>
       <c r="I6" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL6" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="31"/>
+      <c r="B7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG7" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL7" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AL6" s="17" t="s">
+      <c r="AM7" s="12" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:48" ht="84">
-      <c r="A7" s="34"/>
-      <c r="B7" s="12" t="s">
+      <c r="AN7" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="AO7" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="AP7" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="AQ7" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="AR7" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="AS7" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="T7" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="U7" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="V7" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="W7" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="X7" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y7" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z7" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA7" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB7" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC7" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD7" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE7" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="AF7" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG7" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH7" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="AI7" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="AJ7" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="AK7" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="AL7" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="AM7" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="AN7" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="AO7" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="AP7" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="AQ7" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="AR7" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="AS7" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="AT7" s="12"/>
       <c r="AU7" s="12"/>
     </row>
-    <row r="8" spans="1:48" s="13" customFormat="1" ht="198.75">
-      <c r="A8" s="34"/>
+    <row r="8" spans="1:48" s="13" customFormat="1" ht="240" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
       <c r="B8" s="14" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="F8" s="15"/>
       <c r="I8" s="17" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="N8" s="19" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="O8" s="17" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="P8" s="20"/>
       <c r="W8" s="19" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="AJ8" s="17" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="AK8" s="17" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="AM8" s="17" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:48" ht="153.75" customHeight="1">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:48" ht="153.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
       <c r="B9" s="5" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="J9" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="31"/>
-      <c r="Y9" s="31"/>
-      <c r="Z9" s="31"/>
-      <c r="AA9" s="31"/>
+      <c r="J9" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="34"/>
       <c r="AB9" s="26" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="AC9" s="26"/>
       <c r="AD9" s="26"/>
@@ -5060,184 +5060,184 @@
       <c r="AQ9" s="6"/>
       <c r="AR9" s="6"/>
       <c r="AS9" s="6" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:48" ht="363.75">
-      <c r="A10" s="34"/>
+    <row r="10" spans="1:48" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="31"/>
       <c r="B10" s="7" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="F10" s="2"/>
       <c r="H10" s="9" t="s">
-        <v>156</v>
+        <v>120</v>
       </c>
       <c r="J10" s="2"/>
       <c r="L10" s="2"/>
       <c r="N10" s="10" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
       <c r="AH10" s="2"/>
       <c r="AM10" s="9" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="AS10" s="2"/>
     </row>
-    <row r="11" spans="1:48" ht="24">
-      <c r="A11" s="34"/>
+    <row r="11" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="31"/>
       <c r="B11" s="4" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="6" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="U11" s="21" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="V11" s="21" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="W11" s="21" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="X11" s="21" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="Y11" s="21" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="Z11" s="21" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="AA11" s="21" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="AB11" s="21" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="AC11" s="21" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="AD11" s="21" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="AE11" s="21" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="AF11" s="21" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="AG11" s="21" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="AH11" s="21" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="AI11" s="21" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="AJ11" s="21" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="AK11" s="21" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="AL11" s="21" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="AM11" s="21" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="AN11" s="21" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="AO11" s="21" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
       <c r="AP11" s="21" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="AQ11" s="21" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="AR11" s="21" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="AS11" s="21" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
       <c r="AT11" s="21" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="AU11" s="21" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:48" ht="12.75">
-      <c r="A12" s="34"/>
+    <row r="12" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="31"/>
       <c r="B12" s="5" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -5247,55 +5247,55 @@
       <c r="AS12" s="2"/>
       <c r="AT12" s="2"/>
     </row>
-    <row r="13" spans="1:48" ht="253.5">
-      <c r="A13" s="34"/>
+    <row r="13" spans="1:48" ht="300" x14ac:dyDescent="0.2">
+      <c r="A13" s="31"/>
       <c r="B13" s="7" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="F13" s="2"/>
       <c r="P13" s="9" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="AA13" s="2"/>
       <c r="AI13" s="9" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="AJ13" s="9" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="AL13" s="9" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2"/>
       <c r="AS13" s="2"/>
       <c r="AT13" s="2"/>
     </row>
-    <row r="14" spans="1:48" ht="12.75">
-      <c r="A14" s="34"/>
+    <row r="14" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="31"/>
       <c r="B14" s="5" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -5420,45 +5420,45 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:48" ht="188.25">
-      <c r="A15" s="34"/>
+    <row r="15" spans="1:48" ht="204" x14ac:dyDescent="0.2">
+      <c r="A15" s="31"/>
       <c r="B15" s="7" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="9" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="O15" s="9" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
       <c r="S15" s="3"/>
       <c r="V15" s="9" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="AB15" s="3"/>
       <c r="AF15" s="11" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="AJ15" s="9" t="s">
-        <v>192</v>
+        <v>156</v>
       </c>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
@@ -5469,207 +5469,207 @@
       <c r="AT15" s="2"/>
       <c r="AU15" s="2"/>
     </row>
-    <row r="16" spans="1:48" ht="24">
-      <c r="A16" s="34"/>
+    <row r="16" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="31"/>
       <c r="B16" s="4" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="6" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="T16" s="5" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="W16" s="5" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="Y16" s="5" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="Z16" s="5" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="AA16" s="5" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="AB16" s="5" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="AD16" s="5" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="AE16" s="5" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="AF16" s="5" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="AG16" s="5" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="AH16" s="5" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="AL16" s="5" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AM16" s="5" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="AN16" s="5" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="AO16" s="5" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="AP16" s="5" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AQ16" s="5" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AR16" s="5" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AS16" s="5" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="AT16" s="5" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:47" ht="12.75">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:47" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="31"/>
       <c r="B17" s="5" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="V17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="W17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="Y17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="AA17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="AD17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="AE17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="AI17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="AM17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="AP17" s="22" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="AQ17" s="3"/>
       <c r="AR17" s="3"/>
@@ -5677,28 +5677,28 @@
       <c r="AT17" s="3"/>
       <c r="AU17" s="3"/>
     </row>
-    <row r="18" spans="1:47" ht="154.5">
-      <c r="A18" s="34"/>
+    <row r="18" spans="1:47" ht="168" x14ac:dyDescent="0.2">
+      <c r="A18" s="31"/>
       <c r="B18" s="7" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="9" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="Q18" s="9" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="T18" s="2"/>
       <c r="AC18" s="2"/>
@@ -5708,13 +5708,13 @@
       <c r="AT18" s="3"/>
       <c r="AU18" s="3"/>
     </row>
-    <row r="19" spans="1:47" ht="36">
-      <c r="A19" s="34"/>
+    <row r="19" spans="1:47" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="31"/>
       <c r="B19" s="5" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -5731,13 +5731,13 @@
       <c r="AT19" s="3"/>
       <c r="AU19" s="3"/>
     </row>
-    <row r="20" spans="1:47" ht="24">
-      <c r="A20" s="34"/>
+    <row r="20" spans="1:47" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="31"/>
       <c r="B20" s="5" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -5753,145 +5753,145 @@
       <c r="AT20" s="3"/>
       <c r="AU20" s="3"/>
     </row>
-    <row r="21" spans="1:47" ht="24">
-      <c r="A21" s="34"/>
+    <row r="21" spans="1:47" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="31"/>
       <c r="B21" s="4" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="C21" s="4"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="6" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="P21" s="6" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="Q21" s="6" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="S21" s="6" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="T21" s="21" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="U21" s="21" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="V21" s="21" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="W21" s="21" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="X21" s="21" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="Y21" s="21" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="Z21" s="21" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="AA21" s="21" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="AB21" s="21" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="AC21" s="21" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="AD21" s="21" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="AE21" s="21" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="AF21" s="21" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="AG21" s="21" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="AH21" s="21" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="AI21" s="21" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="AJ21" s="21" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="AK21" s="21" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="AL21" s="21" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="AM21" s="21" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="AN21" s="21" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="AO21" s="21" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="AP21" s="21" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="AQ21" s="21" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="AR21" s="21" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="AS21" s="21" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="AT21" s="21" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="AU21" s="21" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:47" ht="36">
-      <c r="A22" s="34"/>
+    <row r="22" spans="1:47" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="31"/>
       <c r="B22" s="4" t="s">
-        <v>220</v>
+        <v>184</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>221</v>
+        <v>185</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -5901,8 +5901,8 @@
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
     </row>
-    <row r="23" spans="1:47" ht="12.75">
-      <c r="A23" s="34"/>
+    <row r="23" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="31"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="E23" s="2"/>
@@ -5910,41 +5910,41 @@
       <c r="AA23" s="2"/>
       <c r="AM23" s="2"/>
     </row>
-    <row r="24" spans="1:47" ht="12.75">
-      <c r="A24" s="34"/>
+    <row r="24" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="31"/>
       <c r="B24" s="4" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:47" ht="264.75">
+    <row r="25" spans="1:47" ht="300" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="R25" s="9" t="s">
-        <v>226</v>
+        <v>190</v>
       </c>
       <c r="AQ25" s="9" t="s">
-        <v>227</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
🚚 Agregar coordenadas a puntos
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos CEPER puntos primera capa.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos CEPER puntos primera capa.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\dev\enflujo\070-cra7\aplicaciones\procesador\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554BCC63-21A0-434B-A04F-D1359FE7B71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CE7A06-07BB-40E4-A411-4BA978358506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39285" yWindow="420" windowWidth="35385" windowHeight="15705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40350" yWindow="750" windowWidth="27795" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,9 +83,6 @@
     <t>Observaciones sobre los datos</t>
   </si>
   <si>
-    <t xml:space="preserve">Plaza Bolivar </t>
-  </si>
-  <si>
     <t xml:space="preserve">Calle 19 </t>
   </si>
   <si>
@@ -3751,6 +3748,9 @@
   </si>
   <si>
     <t>Calle 220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plaza de Bolivar </t>
   </si>
 </sst>
 </file>
@@ -4238,10 +4238,10 @@
   <dimension ref="A1:AV25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AO3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AU5" sqref="AU5"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4330,426 +4330,426 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="AV2" s="1"/>
     </row>
     <row r="3" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="O3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="S3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="W3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="X3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="AA3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="AE3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="W3" s="21" t="s">
+      <c r="AF3" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="X3" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y3" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z3" s="21" t="s">
+      <c r="AG3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH3" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="21" t="s">
+      <c r="AI3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AB3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD3" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE3" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF3" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG3" s="21" t="s">
+      <c r="AJ3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="AH3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI3" s="21" t="s">
+      <c r="AK3" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL3" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO3" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="AJ3" s="21" t="s">
+      <c r="AT3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="AK3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="AL3" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM3" s="21" t="s">
+      <c r="AU3" s="21" t="s">
         <v>32</v>
-      </c>
-      <c r="AN3" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="AO3" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP3" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="AQ3" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="AR3" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="AS3" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="AT3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="AU3" s="21" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="31"/>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="K4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="P4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="R4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="AG4" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="AJ4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" s="6" t="s">
+      <c r="AM4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="AO4" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="S4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y4" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA4" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB4" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC4" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD4" s="21" t="s">
+      <c r="AP4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ4" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR4" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="AE4" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF4" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH4" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI4" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ4" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="AK4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM4" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="AN4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO4" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP4" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ4" s="21" t="s">
+      <c r="AT4" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AR4" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="AT4" s="21" t="s">
+      <c r="AU4" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="AU4" s="21" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:48" s="13" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A5" s="31"/>
       <c r="B5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4757,16 +4757,16 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P5" s="12"/>
       <c r="Q5" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
@@ -4775,13 +4775,13 @@
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
       <c r="AA5" s="12"/>
       <c r="AB5" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC5" s="12"/>
       <c r="AD5" s="12"/>
@@ -4806,158 +4806,158 @@
     <row r="6" spans="1:48" s="13" customFormat="1" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="31"/>
       <c r="B6" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="E6" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="15"/>
       <c r="I6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL6" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="AL6" s="17" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:48" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A7" s="31"/>
       <c r="B7" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="K7" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="L7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="N7" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="O7" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="P7" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="R7" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="S7" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="S7" s="12" t="s">
+      <c r="T7" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="T7" s="12" t="s">
+      <c r="U7" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="U7" s="12" t="s">
+      <c r="V7" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="V7" s="12" t="s">
+      <c r="W7" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="W7" s="12" t="s">
+      <c r="X7" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="X7" s="12" t="s">
+      <c r="Y7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="Y7" s="12" t="s">
+      <c r="Z7" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="Z7" s="12" t="s">
+      <c r="AA7" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="AA7" s="12" t="s">
+      <c r="AB7" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AB7" s="12" t="s">
+      <c r="AC7" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AC7" s="12" t="s">
+      <c r="AD7" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AD7" s="12" t="s">
+      <c r="AE7" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="12" t="s">
+      <c r="AF7" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AF7" s="12" t="s">
+      <c r="AG7" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="AG7" s="12" t="s">
+      <c r="AH7" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="AH7" s="12" t="s">
+      <c r="AI7" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="AI7" s="12" t="s">
+      <c r="AJ7" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="AJ7" s="12" t="s">
+      <c r="AK7" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="AK7" s="12" t="s">
+      <c r="AL7" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AL7" s="12" t="s">
+      <c r="AM7" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AM7" s="12" t="s">
+      <c r="AN7" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="AN7" s="12" t="s">
+      <c r="AO7" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AO7" s="12" t="s">
+      <c r="AP7" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="AP7" s="12" t="s">
+      <c r="AQ7" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="AQ7" s="12" t="s">
+      <c r="AR7" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="AR7" s="12" t="s">
+      <c r="AS7" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="AS7" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="AT7" s="12"/>
       <c r="AU7" s="12"/>
@@ -4965,67 +4965,67 @@
     <row r="8" spans="1:48" s="13" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="31"/>
       <c r="B8" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="E8" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="15"/>
       <c r="I8" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="M8" s="17" t="s">
+      <c r="N8" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="O8" s="17" t="s">
         <v>107</v>
-      </c>
-      <c r="O8" s="17" t="s">
-        <v>108</v>
       </c>
       <c r="P8" s="20"/>
       <c r="W8" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ8" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="AJ8" s="17" t="s">
+      <c r="AK8" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="AK8" s="17" t="s">
+      <c r="AM8" s="17" t="s">
         <v>111</v>
-      </c>
-      <c r="AM8" s="17" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:48" ht="153.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="31"/>
       <c r="B9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="D9" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="2"/>
       <c r="J9" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K9" s="33"/>
       <c r="L9" s="33"/>
       <c r="M9" s="33"/>
       <c r="N9" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
@@ -5041,7 +5041,7 @@
       <c r="Z9" s="34"/>
       <c r="AA9" s="34"/>
       <c r="AB9" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AC9" s="26"/>
       <c r="AD9" s="26"/>
@@ -5060,184 +5060,184 @@
       <c r="AQ9" s="6"/>
       <c r="AR9" s="6"/>
       <c r="AS9" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:48" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A10" s="31"/>
       <c r="B10" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
-        <v>59</v>
-      </c>
       <c r="E10" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" s="2"/>
       <c r="H10" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J10" s="2"/>
       <c r="L10" s="2"/>
       <c r="N10" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AH10" s="2"/>
       <c r="AM10" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AS10" s="2"/>
     </row>
     <row r="11" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="31"/>
       <c r="B11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="M11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="P11" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="K11" s="6" t="s">
+      <c r="Q11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="S11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="T11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U11" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="V11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="W11" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="X11" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y11" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z11" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="M11" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="R11" s="6" t="s">
+      <c r="AA11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB11" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC11" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="S11" s="6" t="s">
+      <c r="AD11" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE11" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF11" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG11" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH11" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI11" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ11" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK11" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="T11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="U11" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="V11" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="W11" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="X11" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y11" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z11" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA11" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB11" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC11" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="AD11" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="AE11" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="AF11" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="AG11" s="21" t="s">
+      <c r="AM11" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="AH11" s="21" t="s">
+      <c r="AN11" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="AO11" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP11" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="AI11" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ11" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="AK11" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="AL11" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM11" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="AN11" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="AO11" s="21" t="s">
+      <c r="AQ11" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="AP11" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="AQ11" s="21" t="s">
+      <c r="AR11" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AS11" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="AR11" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="AS11" s="21" t="s">
+      <c r="AT11" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="AT11" s="21" t="s">
+      <c r="AU11" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="AU11" s="21" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="31"/>
       <c r="B12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -5250,36 +5250,36 @@
     <row r="13" spans="1:48" ht="300" x14ac:dyDescent="0.2">
       <c r="A13" s="31"/>
       <c r="B13" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
-        <v>59</v>
-      </c>
       <c r="E13" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2"/>
       <c r="P13" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q13" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="W13" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="W13" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="AA13" s="2"/>
       <c r="AI13" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ13" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="AJ13" s="9" t="s">
+      <c r="AL13" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="AL13" s="9" t="s">
-        <v>148</v>
       </c>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2"/>
@@ -5289,13 +5289,13 @@
     <row r="14" spans="1:48" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="31"/>
       <c r="B14" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -5423,42 +5423,42 @@
     <row r="15" spans="1:48" ht="204" x14ac:dyDescent="0.2">
       <c r="A15" s="31"/>
       <c r="B15" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
         <v>58</v>
       </c>
-      <c r="D15" t="s">
-        <v>59</v>
-      </c>
       <c r="E15" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>150</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>151</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="O15" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q15" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="Q15" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="S15" s="3"/>
       <c r="V15" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB15" s="3"/>
       <c r="AF15" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AJ15" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="AJ15" s="9" t="s">
-        <v>156</v>
       </c>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
@@ -5472,204 +5472,204 @@
     <row r="16" spans="1:48" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="31"/>
       <c r="B16" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="U16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="O16" s="5" t="s">
+      <c r="V16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="P16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="U16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="V16" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="W16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z16" s="5" t="s">
+      <c r="AC16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AA16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG16" s="5" t="s">
+      <c r="AI16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AM16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AH16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AK16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL16" s="5" t="s">
+      <c r="AN16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AM16" s="5" t="s">
+      <c r="AO16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AN16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AO16" s="5" t="s">
+      <c r="AP16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AP16" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="AQ16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AR16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AS16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AT16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:47" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="31"/>
       <c r="B17" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="V17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="W17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Y17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AA17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AD17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AE17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AI17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AM17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AP17" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AQ17" s="3"/>
       <c r="AR17" s="3"/>
@@ -5680,25 +5680,25 @@
     <row r="18" spans="1:47" ht="168" x14ac:dyDescent="0.2">
       <c r="A18" s="31"/>
       <c r="B18" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
       <c r="E18" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="Q18" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T18" s="2"/>
       <c r="AC18" s="2"/>
@@ -5711,10 +5711,10 @@
     <row r="19" spans="1:47" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="31"/>
       <c r="B19" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -5734,10 +5734,10 @@
     <row r="20" spans="1:47" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="31"/>
       <c r="B20" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -5756,142 +5756,142 @@
     <row r="21" spans="1:47" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="31"/>
       <c r="B21" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" s="4"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H21" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="I21" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="J21" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="J21" s="6" t="s">
+      <c r="K21" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="L21" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="M21" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="S21" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="L21" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="M21" s="6" t="s">
+      <c r="T21" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="U21" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="V21" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="W21" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="X21" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y21" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z21" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA21" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB21" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="N21" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="O21" s="6" t="s">
+      <c r="AC21" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="P21" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q21" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="R21" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="S21" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="T21" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="U21" s="21" t="s">
+      <c r="AD21" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="AE21" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="AF21" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG21" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH21" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="AI21" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="AJ21" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="AK21" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="AL21" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="AM21" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="AN21" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="V21" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="W21" s="21" t="s">
+      <c r="AO21" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="AP21" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="AQ21" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="AR21" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="AS21" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="X21" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y21" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="Z21" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA21" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="AB21" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC21" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="AD21" s="21" t="s">
+      <c r="AT21" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="AE21" s="21" t="s">
+      <c r="AU21" s="21" t="s">
         <v>180</v>
-      </c>
-      <c r="AF21" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="AG21" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="AH21" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="AI21" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="AJ21" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="AK21" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="AL21" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="AM21" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="AN21" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="AO21" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="AP21" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="AQ21" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="AR21" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="AS21" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="AT21" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="AU21" s="21" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:47" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="31"/>
       <c r="B22" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -5913,38 +5913,38 @@
     <row r="24" spans="1:47" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="31"/>
       <c r="B24" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>187</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:47" ht="300" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
         <v>58</v>
       </c>
-      <c r="D25" t="s">
-        <v>59</v>
-      </c>
       <c r="E25" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H25" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q25" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="Q25" s="9" t="s">
+      <c r="R25" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="R25" s="9" t="s">
+      <c r="AQ25" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="AQ25" s="9" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✅ Agregar índice de caminabilidad
</commit_message>
<xml_diff>
--- a/aplicaciones/procesador/datos/Mapa 7ma - Datos CEPER puntos primera capa.xlsx
+++ b/aplicaciones/procesador/datos/Mapa 7ma - Datos CEPER puntos primera capa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/la_guzman_uniandes_edu_co/Documents/Corredor Verde 7/Diseminación de resultados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="14_{7DCA08D4-326D-405B-9417-42839C200435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B74C0B20-8A95-4B6E-B58F-01520221D790}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75178097-8B55-4694-817C-9DBDF1177FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="243">
   <si>
     <t>TRAMOS</t>
   </si>
@@ -3636,6 +3636,9 @@
   </si>
   <si>
     <t>"Aquí porque queda el Hospital Simón Bolívar y el complejo de Servitá, que son lugares importantes. Es un Hospital donde viene mucha mucha gente y también un Centro Cultural el de Servitá, donde pasan muchas cosas. Vienen adultos mayores, hay una biblioteca, viene gente a leer, a estudiar, gente que la única posibilidad que tienes es venir aquí a Servitá. Obviamente al Hospital Simón Bolívar le aquejan todos los problemas de lo público; hay gente que espera muchísimo tiempo, gente que no tiene la mejor atención pero es un punto importante. Además de esto, por ejemplo, este hospital está en contraposición a otro hospital que es la Santa Fe. Que es un hospital totalmente diferente a este. "</t>
+  </si>
+  <si>
+    <t>Caminabilidad</t>
   </si>
   <si>
     <t>I. Caminabilidad</t>
@@ -3902,7 +3905,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3924,6 +3927,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3977,7 +3986,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4039,7 +4048,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4054,17 +4072,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -4302,8 +4314,8 @@
   <dimension ref="A1:AV25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="AO3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="AV6" sqref="AV6"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="B14:C14"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -4327,53 +4339,53 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="23" t="s">
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="23" t="s">
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="32"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="26"/>
       <c r="AV1" s="1"/>
     </row>
     <row r="2" spans="1:48" ht="26.25" customHeight="1">
@@ -4519,7 +4531,7 @@
       <c r="AV2" s="1"/>
     </row>
     <row r="3" spans="1:48" ht="23.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -4660,7 +4672,7 @@
       </c>
     </row>
     <row r="4" spans="1:48" ht="23.25">
-      <c r="A4" s="33"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="4" t="s">
         <v>69</v>
       </c>
@@ -4799,7 +4811,7 @@
       </c>
     </row>
     <row r="5" spans="1:48" s="13" customFormat="1" ht="69">
-      <c r="A5" s="33"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="12" t="s">
         <v>84</v>
       </c>
@@ -4868,7 +4880,7 @@
       <c r="AU5" s="12"/>
     </row>
     <row r="6" spans="1:48" s="13" customFormat="1" ht="171.75">
-      <c r="A6" s="33"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="14" t="s">
         <v>84</v>
       </c>
@@ -4890,7 +4902,7 @@
       </c>
     </row>
     <row r="7" spans="1:48" ht="81">
-      <c r="A7" s="33"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="12" t="s">
         <v>98</v>
       </c>
@@ -5027,7 +5039,7 @@
       <c r="AU7" s="12"/>
     </row>
     <row r="8" spans="1:48" s="13" customFormat="1" ht="192.75">
-      <c r="A8" s="33"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="14" t="s">
         <v>140</v>
       </c>
@@ -5068,7 +5080,7 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="153.75" customHeight="1">
-      <c r="A9" s="33"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="5" t="s">
         <v>149</v>
       </c>
@@ -5082,39 +5094,39 @@
         <v>99</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="25" t="s">
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
-      <c r="AA9" s="27"/>
-      <c r="AB9" s="30" t="s">
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30"/>
+      <c r="AB9" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="AC9" s="30"/>
-      <c r="AD9" s="30"/>
-      <c r="AE9" s="30"/>
-      <c r="AF9" s="30"/>
-      <c r="AG9" s="30"/>
-      <c r="AH9" s="30"/>
-      <c r="AI9" s="30"/>
-      <c r="AJ9" s="30"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="23"/>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
+      <c r="AH9" s="23"/>
+      <c r="AI9" s="23"/>
+      <c r="AJ9" s="23"/>
       <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
       <c r="AM9" s="6"/>
@@ -5128,7 +5140,7 @@
       </c>
     </row>
     <row r="10" spans="1:48" ht="353.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="7" t="s">
         <v>155</v>
       </c>
@@ -5157,7 +5169,7 @@
       <c r="AS10" s="2"/>
     </row>
     <row r="11" spans="1:48" ht="23.25">
-      <c r="A11" s="33"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="4" t="s">
         <v>159</v>
       </c>
@@ -5296,7 +5308,7 @@
       </c>
     </row>
     <row r="12" spans="1:48" ht="12.75">
-      <c r="A12" s="33"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="5" t="s">
         <v>182</v>
       </c>
@@ -5312,7 +5324,7 @@
       <c r="AT12" s="2"/>
     </row>
     <row r="13" spans="1:48" ht="246.75">
-      <c r="A13" s="33"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="7" t="s">
         <v>182</v>
       </c>
@@ -5351,11 +5363,11 @@
       <c r="AT13" s="2"/>
     </row>
     <row r="14" spans="1:48" ht="12.75">
-      <c r="A14" s="33"/>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="31" t="s">
         <v>183</v>
       </c>
       <c r="D14" t="s">
@@ -5485,9 +5497,9 @@
       </c>
     </row>
     <row r="15" spans="1:48" ht="182.25">
-      <c r="A15" s="33"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>94</v>
@@ -5500,29 +5512,29 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="O15" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="S15" s="3"/>
       <c r="V15" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AB15" s="3"/>
       <c r="AF15" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AJ15" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
@@ -5534,9 +5546,9 @@
       <c r="AU15" s="2"/>
     </row>
     <row r="16" spans="1:48" ht="23.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>52</v>
@@ -5552,7 +5564,7 @@
         <v>64</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>73</v>
@@ -5564,22 +5576,22 @@
         <v>78</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="N16" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="P16" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="O16" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>200</v>
-      </c>
       <c r="Q16" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="R16" s="5" t="s">
         <v>81</v>
@@ -5606,7 +5618,7 @@
         <v>57</v>
       </c>
       <c r="Z16" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AA16" s="5" t="s">
         <v>59</v>
@@ -5633,25 +5645,25 @@
         <v>57</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AL16" s="5" t="s">
         <v>77</v>
       </c>
       <c r="AM16" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AN16" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="AN16" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="AO16" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AP16" s="5" t="s">
         <v>77</v>
@@ -5666,16 +5678,16 @@
         <v>77</v>
       </c>
       <c r="AT16" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:47" ht="12.75">
-      <c r="A17" s="33"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>52</v>
@@ -5684,59 +5696,59 @@
       <c r="F17" s="2"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="V17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="W17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Y17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AA17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AC17" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AD17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AE17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AI17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AM17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AP17" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AQ17" s="3"/>
       <c r="AR17" s="3"/>
@@ -5745,9 +5757,9 @@
       <c r="AU17" s="3"/>
     </row>
     <row r="18" spans="1:47" ht="150.75">
-      <c r="A18" s="33"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>94</v>
@@ -5760,12 +5772,12 @@
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="Q18" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="T18" s="2"/>
       <c r="AC18" s="2"/>
@@ -5776,9 +5788,9 @@
       <c r="AU18" s="3"/>
     </row>
     <row r="19" spans="1:47" ht="35.25">
-      <c r="A19" s="33"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>52</v>
@@ -5799,9 +5811,9 @@
       <c r="AU19" s="3"/>
     </row>
     <row r="20" spans="1:47" ht="23.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>52</v>
@@ -5821,9 +5833,9 @@
       <c r="AU20" s="3"/>
     </row>
     <row r="21" spans="1:47" ht="23.25">
-      <c r="A21" s="33"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" t="s">
@@ -5834,136 +5846,136 @@
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="21" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I21" s="21" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J21" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="K21" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="M21" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="N21" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="O21" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="P21" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q21" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="R21" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="S21" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="K21" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="L21" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="M21" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="N21" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="O21" s="21" t="s">
+      <c r="T21" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="U21" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="V21" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="W21" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="X21" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y21" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z21" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA21" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="AB21" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="P21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q21" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="R21" s="21" t="s">
+      <c r="AC21" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="S21" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="T21" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="U21" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="V21" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="W21" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="X21" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="Y21" s="21" t="s">
+      <c r="AD21" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="AE21" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="AF21" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="AG21" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH21" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="AI21" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="AJ21" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="AK21" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="AL21" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="AM21" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="AN21" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="Z21" s="21" t="s">
+      <c r="AO21" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="AP21" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="AQ21" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="AR21" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="AS21" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="AA21" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="AB21" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="AC21" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD21" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE21" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF21" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="AG21" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="AH21" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="AI21" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="AJ21" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="AK21" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="AL21" s="21" t="s">
+      <c r="AT21" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="AM21" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="AN21" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="AO21" s="21" t="s">
+      <c r="AU21" s="21" t="s">
         <v>232</v>
-      </c>
-      <c r="AP21" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="AQ21" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="AR21" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="AS21" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="AT21" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="AU21" s="21" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:47" ht="35.25">
-      <c r="A22" s="33"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -5974,7 +5986,7 @@
       <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:47" ht="12.75">
-      <c r="A23" s="33"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="E23" s="2"/>
@@ -5983,19 +5995,19 @@
       <c r="AM23" s="2"/>
     </row>
     <row r="24" spans="1:47" ht="12.75">
-      <c r="A24" s="33"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:47" ht="257.25">
       <c r="B25" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>94</v>
@@ -6007,16 +6019,16 @@
         <v>87</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="R25" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AQ25" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>